<commit_message>
.csv files stop at first blank row.  Event filenames are two digit.
Calendar sheet renamed to calendar as expected by python script.
</commit_message>
<xml_diff>
--- a/data/ClubEvents_2026.xlsx
+++ b/data/ClubEvents_2026.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\wvcc\WellandValleyCC.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240D78D7-E7CE-447D-8A0F-3AFBA73554E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD61B69-1F4D-4859-A31D-AB11684FC20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="7" xr2:uid="{45F9DFA6-3E60-47DF-96C3-C485FAB93508}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{45F9DFA6-3E60-47DF-96C3-C485FAB93508}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisions" sheetId="1" r:id="rId1"/>
     <sheet name="competitors" sheetId="31" r:id="rId2"/>
-    <sheet name="Calendar" sheetId="2" r:id="rId3"/>
+    <sheet name="calendar" sheetId="2" r:id="rId3"/>
     <sheet name="RoundRobinRiders" sheetId="4" r:id="rId4"/>
     <sheet name="Event (1)" sheetId="5" r:id="rId5"/>
     <sheet name="Event (2)" sheetId="6" r:id="rId6"/>
@@ -45,52 +45,52 @@
     <sheet name="Event (26)" sheetId="30" r:id="rId30"/>
   </sheets>
   <definedNames>
-    <definedName name="ActualPCN">Calendar!$D$52</definedName>
-    <definedName name="BestNumberOfEvents">Calendar!$D$36</definedName>
-    <definedName name="Calendar">Calendar!$A$4:$F$31</definedName>
-    <definedName name="CalendarEventNumbers">Calendar!$A$4:$A$31</definedName>
-    <definedName name="CalendarNumberOfCompetitors">Calendar!$H$4:$H$31</definedName>
+    <definedName name="ActualPCN">calendar!$D$52</definedName>
+    <definedName name="BestNumberOfEvents">calendar!$D$36</definedName>
+    <definedName name="Calendar">calendar!$A$4:$F$31</definedName>
+    <definedName name="CalendarEventNumbers">calendar!$A$4:$A$31</definedName>
+    <definedName name="CalendarNumberOfCompetitors">calendar!$H$4:$H$31</definedName>
     <definedName name="CompetitionNames">#REF!</definedName>
     <definedName name="CompetitionNumbers">#REF!</definedName>
-    <definedName name="CompetitionYear">Calendar!$D$33</definedName>
+    <definedName name="CompetitionYear">calendar!$D$33</definedName>
     <definedName name="DCR">#REF!</definedName>
     <definedName name="DistanceNewVS">#REF!</definedName>
-    <definedName name="EDPrefix">Calendar!$D$47</definedName>
-    <definedName name="EDSuffix">Calendar!$D$48</definedName>
-    <definedName name="ESPrefix">Calendar!$D$50</definedName>
-    <definedName name="ESSuffix">Calendar!$D$51</definedName>
-    <definedName name="Event">Calendar!$D$34</definedName>
-    <definedName name="EventDateTimes">Calendar!$G$4:$G$30</definedName>
-    <definedName name="EventJunColumn">Calendar!$D$67</definedName>
-    <definedName name="EventJuvColumn">Calendar!$D$66</definedName>
-    <definedName name="EventsCompletedToDate">Calendar!$D$38</definedName>
-    <definedName name="GenderColumn">Calendar!$D$62</definedName>
+    <definedName name="EDPrefix">calendar!$D$47</definedName>
+    <definedName name="EDSuffix">calendar!$D$48</definedName>
+    <definedName name="ESPrefix">calendar!$D$50</definedName>
+    <definedName name="ESSuffix">calendar!$D$51</definedName>
+    <definedName name="Event">calendar!$D$34</definedName>
+    <definedName name="EventDateTimes">calendar!$G$4:$G$30</definedName>
+    <definedName name="EventJunColumn">calendar!$D$67</definedName>
+    <definedName name="EventJuvColumn">calendar!$D$66</definedName>
+    <definedName name="EventsCompletedToDate">calendar!$D$38</definedName>
+    <definedName name="GenderColumn">calendar!$D$62</definedName>
     <definedName name="IDsNewVS">#REF!</definedName>
     <definedName name="JunCol">#REF!</definedName>
-    <definedName name="JunColumn">Calendar!$D$64</definedName>
-    <definedName name="JunPCN">Calendar!$D$59</definedName>
-    <definedName name="JuvColumn">Calendar!$D$63</definedName>
-    <definedName name="JuvPCN">Calendar!$D$58</definedName>
-    <definedName name="LeagueSponsor">Calendar!$D$44</definedName>
-    <definedName name="MaximumScorePerEvent">Calendar!$D$39</definedName>
-    <definedName name="MaxScoreFromRemainingEvents">Calendar!$D$41</definedName>
+    <definedName name="JunColumn">calendar!$D$64</definedName>
+    <definedName name="JunPCN">calendar!$D$59</definedName>
+    <definedName name="JuvColumn">calendar!$D$63</definedName>
+    <definedName name="JuvPCN">calendar!$D$58</definedName>
+    <definedName name="LeagueSponsor">calendar!$D$44</definedName>
+    <definedName name="MaximumScorePerEvent">calendar!$D$39</definedName>
+    <definedName name="MaxScoreFromRemainingEvents">calendar!$D$41</definedName>
     <definedName name="MemberData">'Event (1)'!$G$2</definedName>
     <definedName name="MemberDataCC">#REF!</definedName>
     <definedName name="NameToNumber">#REF!</definedName>
-    <definedName name="nChampionshipEventsCancelled">Calendar!$I$33</definedName>
-    <definedName name="NevBrooksBestNumberOfEvents">Calendar!$D$37</definedName>
+    <definedName name="nChampionshipEventsCancelled">calendar!$I$33</definedName>
+    <definedName name="NevBrooksBestNumberOfEvents">calendar!$D$37</definedName>
     <definedName name="NevBrooksHandicapTable">#REF!</definedName>
-    <definedName name="NevBrooksPCN">Calendar!$D$60</definedName>
-    <definedName name="NevBrooksStandardTime">Calendar!$D$43</definedName>
-    <definedName name="nEvening10Events">Calendar!$K$32</definedName>
-    <definedName name="nEvening10EventsCancelled">Calendar!$K$33</definedName>
+    <definedName name="NevBrooksPCN">calendar!$D$60</definedName>
+    <definedName name="NevBrooksStandardTime">calendar!$D$43</definedName>
+    <definedName name="nEvening10Events">calendar!$K$32</definedName>
+    <definedName name="nEvening10EventsCancelled">calendar!$K$33</definedName>
     <definedName name="NewVSMen">#REF!</definedName>
     <definedName name="NewVSWomen">#REF!</definedName>
-    <definedName name="NonTenEvents">Calendar!$J$4:$J$30</definedName>
-    <definedName name="NumberOfForcedScores">Calendar!$D$40</definedName>
+    <definedName name="NonTenEvents">calendar!$J$4:$J$30</definedName>
+    <definedName name="NumberOfForcedScores">calendar!$D$40</definedName>
     <definedName name="NumberToDivision">#REF!</definedName>
     <definedName name="Points">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Calendar!$B$1:$H$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">calendar!$B$1:$H$30</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Event (1)'!$G$1:$H$22</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">'Event (10)'!$G$1:$H$31</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="14">'Event (11)'!$G$1:$H$27</definedName>
@@ -118,21 +118,21 @@
     <definedName name="_xlnm.Print_Area" localSheetId="11">'Event (8)'!$G$1:$H$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">'Event (9)'!$G$1:$H$16</definedName>
     <definedName name="PublishRange">#REF!,#REF!,#REF!</definedName>
-    <definedName name="RoadMenPCN">Calendar!$D$56</definedName>
-    <definedName name="RoadWomenPCN">Calendar!$D$57</definedName>
+    <definedName name="RoadMenPCN">calendar!$D$56</definedName>
+    <definedName name="RoadWomenPCN">calendar!$D$57</definedName>
     <definedName name="RoundRobinNameToClub">RoundRobinRiders!$A$2:$C$32</definedName>
     <definedName name="RoundRobinNameToClubRange">RoundRobinRiders!$A$2:$C$132</definedName>
-    <definedName name="SenPCN">Calendar!$D$53</definedName>
+    <definedName name="SenPCN">calendar!$D$53</definedName>
     <definedName name="SnrFCData">#REF!</definedName>
     <definedName name="SortRangeForWVCCData">#REF!</definedName>
-    <definedName name="SponsorMessage">Calendar!$D$45</definedName>
+    <definedName name="SponsorMessage">calendar!$D$45</definedName>
     <definedName name="StandardsMen">#REF!</definedName>
     <definedName name="StandardsWomen">#REF!</definedName>
-    <definedName name="TenMileEvents">Calendar!$K$4:$K$31</definedName>
-    <definedName name="TotalNumberOfEvents">Calendar!$D$35</definedName>
-    <definedName name="VetPCN">Calendar!$D$55</definedName>
-    <definedName name="VetsMinimumAge">Calendar!$D$42</definedName>
-    <definedName name="WomPCN">Calendar!$D$54</definedName>
+    <definedName name="TenMileEvents">calendar!$K$4:$K$31</definedName>
+    <definedName name="TotalNumberOfEvents">calendar!$D$35</definedName>
+    <definedName name="VetPCN">calendar!$D$55</definedName>
+    <definedName name="VetsMinimumAge">calendar!$D$42</definedName>
+    <definedName name="WomPCN">calendar!$D$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48723,8 +48723,8 @@
   </sheetPr>
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C298" sqref="C298"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -59192,7 +59192,7 @@
   </sheetPr>
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trigger pipeline with ClubEvents_YYYY.xlsx update
</commit_message>
<xml_diff>
--- a/data/ClubEvents_2026.xlsx
+++ b/data/ClubEvents_2026.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\wvcc\WellandValleyCC.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0532F9D3-5D87-4BE1-8D67-943FA2B1632D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718C274F-CED0-4B82-B974-5DAA3EA762E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="2" xr2:uid="{45F9DFA6-3E60-47DF-96C3-C485FAB93508}"/>
   </bookViews>
@@ -48730,7 +48730,7 @@
   <cols>
     <col min="1" max="1" width="11.86328125" style="10" customWidth="1"/>
     <col min="2" max="2" width="15.3984375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="12" customWidth="1"/>
     <col min="4" max="4" width="31.53125" style="12" customWidth="1"/>
     <col min="5" max="5" width="8" style="10" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" style="12" bestFit="1" customWidth="1"/>

</xml_diff>